<commit_message>
Fix 'k' column to be more general -> Power_WeightsK v0.1.1
</commit_message>
<xml_diff>
--- a/examples/Power_WeightsK.xlsx
+++ b/examples/Power_WeightsK.xlsx
@@ -614,7 +614,7 @@
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>v0.1.0</t>
+          <t>v0.1.1</t>
         </is>
       </c>
     </row>
@@ -680,7 +680,7 @@
       </c>
       <c r="C5" s="7" t="inlineStr">
         <is>
-          <t>Representative hour in rp for this hour</t>
+          <t>Representative hour within rp</t>
         </is>
       </c>
       <c r="D5" s="7" t="inlineStr">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>v0.1.0</t>
+          <t>v0.1.1</t>
         </is>
       </c>
     </row>
@@ -1423,7 +1423,7 @@
       </c>
       <c r="C5" s="7" t="inlineStr">
         <is>
-          <t>Representative hour in rp for this hour</t>
+          <t>Representative hour within rp</t>
         </is>
       </c>
       <c r="D5" s="7" t="inlineStr">

</xml_diff>

<commit_message>
Implement writing of Power_ThermalGen -> v0.1.0
Fix formatting of pWeight_rp/k (and update Power_WeightsRP/K -> v0.1.2)
Improve error messages in compare_Excels
</commit_message>
<xml_diff>
--- a/examples/Power_WeightsK.xlsx
+++ b/examples/Power_WeightsK.xlsx
@@ -17,7 +17,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="6">
     <font>
       <name val="Calibri"/>
@@ -133,7 +135,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -614,7 +616,7 @@
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>v0.1.1</t>
+          <t>v0.1.2</t>
         </is>
       </c>
     </row>
@@ -1357,7 +1359,7 @@
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>v0.1.1</t>
+          <t>v0.1.2</t>
         </is>
       </c>
     </row>

</xml_diff>